<commit_message>
mise à jour SCRUM 06
</commit_message>
<xml_diff>
--- a/SCRUM/burndown_charts.xlsx
+++ b/SCRUM/burndown_charts.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="44">
   <si>
     <t xml:space="preserve">SPRINT1</t>
   </si>
@@ -824,11 +824,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="53098013"/>
-        <c:axId val="21939174"/>
+        <c:axId val="96946812"/>
+        <c:axId val="59085036"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="53098013"/>
+        <c:axId val="96946812"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -884,7 +884,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21939174"/>
+        <c:crossAx val="59085036"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -892,7 +892,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="21939174"/>
+        <c:axId val="59085036"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -957,7 +957,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53098013"/>
+        <c:crossAx val="96946812"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1198,10 +1198,10 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1216,11 +1216,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="26763654"/>
-        <c:axId val="31445639"/>
+        <c:axId val="34471642"/>
+        <c:axId val="75286770"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="26763654"/>
+        <c:axId val="34471642"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1276,7 +1276,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31445639"/>
+        <c:crossAx val="75286770"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1284,7 +1284,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="31445639"/>
+        <c:axId val="75286770"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1349,7 +1349,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26763654"/>
+        <c:crossAx val="34471642"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1387,9 +1387,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>6120</xdr:colOff>
+      <xdr:colOff>5760</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>52200</xdr:rowOff>
+      <xdr:rowOff>51840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1398,7 +1398,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="460080" y="3657960"/>
-        <a:ext cx="7219080" cy="4059720"/>
+        <a:ext cx="7218720" cy="4059360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1417,9 +1417,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>6120</xdr:colOff>
+      <xdr:colOff>5760</xdr:colOff>
       <xdr:row>72</xdr:row>
-      <xdr:rowOff>61200</xdr:rowOff>
+      <xdr:rowOff>60840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1428,7 +1428,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="460080" y="10308960"/>
-        <a:ext cx="7219080" cy="4016160"/>
+        <a:ext cx="7218720" cy="4015800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1448,8 +1448,8 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G46" activeCellId="0" sqref="G46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B80" activeCellId="0" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1457,8 +1457,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="81.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="3" style="0" width="9.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="5.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="4.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="6.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="4.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="2.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="1.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1018" style="0" width="9.14"/>
   </cols>
   <sheetData>
@@ -1950,8 +1952,8 @@
       <c r="D46" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="E46" s="8" t="s">
-        <v>36</v>
+      <c r="E46" s="8" t="n">
+        <v>4</v>
       </c>
       <c r="F46" s="9"/>
       <c r="G46" s="2"/>
@@ -2025,7 +2027,7 @@
         <v>5</v>
       </c>
       <c r="E49" s="8" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F49" s="9"/>
       <c r="G49" s="18" t="n">
@@ -2037,12 +2039,12 @@
         <v>10</v>
       </c>
       <c r="I49" s="18" t="n">
-        <f aca="false">D50+D49+D45</f>
-        <v>15</v>
+        <f aca="false">D44</f>
+        <v>3</v>
       </c>
       <c r="J49" s="18" t="n">
-        <f aca="false">D46</f>
-        <v>3</v>
+        <f aca="false">D46+D49+D50</f>
+        <v>13</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2057,7 +2059,7 @@
         <v>5</v>
       </c>
       <c r="E50" s="8" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F50" s="9"/>
     </row>
@@ -2168,11 +2170,11 @@
       </c>
       <c r="F68" s="25" t="n">
         <f aca="false">E68-I49</f>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="G68" s="25" t="n">
         <f aca="false">F68-J49</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>